<commit_message>
ages minimum and maximum added
</commit_message>
<xml_diff>
--- a/Dataset/BVC_Voice_Bio_Public.xlsx
+++ b/Dataset/BVC_Voice_Bio_Public.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m4ria\OneDrive\Documentos\4ano\DACO\ProjetoDACO\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FED9B10-BB21-4934-AF95-2A6FA11638B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD8B9E7-F218-4F2C-8405-A6BAA03F3C49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{257983B8-A270-084B-BEBA-A148FAD49B75}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="45">
   <si>
     <t>New_ID</t>
   </si>
@@ -158,6 +158,18 @@
   <si>
     <t>'Okirika'</t>
   </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Subconjuntos de Idades</t>
+  </si>
+  <si>
+    <t>Matos</t>
+  </si>
 </sst>
 </file>
 
@@ -206,10 +218,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,15 +542,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B819E7F-6A5B-3540-96F7-866BED53D692}">
-  <dimension ref="A1:F561"/>
+  <dimension ref="A1:K561"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,8 +563,13 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="I1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4001</v>
       </c>
@@ -563,8 +586,20 @@
         <f>COUNTIF(B2:B527,"='Male'")</f>
         <v>336</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2">
+        <f>MIN(C2:C561)</f>
+        <v>14</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4002</v>
       </c>
@@ -581,8 +616,15 @@
         <f>COUNTIF(B2:B527,"='Female'")</f>
         <v>190</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3">
+        <f>MAX(C2:C561)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4003</v>
       </c>
@@ -596,7 +638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4004</v>
       </c>
@@ -613,7 +655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4005</v>
       </c>
@@ -630,7 +672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4006</v>
       </c>
@@ -647,7 +689,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4007</v>
       </c>
@@ -664,7 +706,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4008</v>
       </c>
@@ -681,7 +723,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>4010</v>
       </c>
@@ -698,7 +740,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>4011</v>
       </c>
@@ -712,7 +754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>4012</v>
       </c>
@@ -726,7 +768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4020</v>
       </c>
@@ -740,7 +782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>4021</v>
       </c>
@@ -754,7 +796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>4022</v>
       </c>
@@ -768,7 +810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>4026</v>
       </c>
@@ -8413,6 +8455,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="57" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>